<commit_message>
added team acronyms and more plot trials
</commit_message>
<xml_diff>
--- a/code/data/Edge_List_Transfers.xlsx
+++ b/code/data/Edge_List_Transfers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienlattmann/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\Studium\Master\4_Semester\MethodenDerSozialenNetzwerke\Project\SocialNetworkAnalysis\social_network_analysis\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF27EB3-B75C-164B-B1C0-256739D3CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A785E174-2D96-4BAA-8F3A-A5A7C07E1DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1320" windowWidth="28980" windowHeight="18820" xr2:uid="{FABA5661-431C-7B4B-8938-D299ED5A487A}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="12735" xr2:uid="{FABA5661-431C-7B4B-8938-D299ED5A487A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="47">
   <si>
     <t>Kürzel x</t>
   </si>
@@ -106,6 +107,75 @@
   </si>
   <si>
     <t>FC Winterhur</t>
+  </si>
+  <si>
+    <t>YB</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>BAS</t>
+  </si>
+  <si>
+    <t>LUG</t>
+  </si>
+  <si>
+    <t>LUZ</t>
+  </si>
+  <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>VAD</t>
+  </si>
+  <si>
+    <t>THU</t>
+  </si>
+  <si>
+    <t>AAR</t>
+  </si>
+  <si>
+    <t>WIN</t>
+  </si>
+  <si>
+    <t>XAM</t>
+  </si>
+  <si>
+    <t>SFC</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>FCZ</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>SLO</t>
+  </si>
+  <si>
+    <t>FCS</t>
+  </si>
+  <si>
+    <t>WILL</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>YS</t>
+  </si>
+  <si>
+    <t>Acronym</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -463,20 +533,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ACF79-FBB0-FD4B-BB40-44B82F9281BB}">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +559,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -511,8 +590,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -533,8 +615,11 @@
       <c r="I3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -555,8 +640,11 @@
       <c r="I4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -577,8 +665,11 @@
       <c r="I5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -599,8 +690,11 @@
       <c r="I6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -621,8 +715,11 @@
       <c r="I7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -643,8 +740,11 @@
       <c r="I8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -665,8 +765,11 @@
       <c r="I9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -687,8 +790,11 @@
       <c r="I10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -709,8 +815,11 @@
       <c r="I11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -731,8 +840,11 @@
       <c r="I12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -753,8 +865,11 @@
       <c r="I13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -775,8 +890,11 @@
       <c r="I14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -797,8 +915,11 @@
       <c r="I15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -819,8 +940,11 @@
       <c r="I16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -841,8 +965,11 @@
       <c r="I17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -863,8 +990,11 @@
       <c r="I18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -885,8 +1015,11 @@
       <c r="I19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -907,8 +1040,11 @@
       <c r="I20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -929,8 +1065,11 @@
       <c r="I21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -946,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -962,7 +1101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -978,7 +1117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -994,7 +1133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1042,7 +1181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1074,7 +1213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +1245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1138,7 +1277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1154,7 +1293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1186,7 +1325,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1202,7 +1341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1218,7 +1357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -1234,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1250,7 +1389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1421,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1298,7 +1437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1314,7 +1453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -1346,7 +1485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -1362,7 +1501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -1378,7 +1517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -1394,7 +1533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -1410,7 +1549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -1426,7 +1565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -1442,7 +1581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1458,7 +1597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -1474,7 +1613,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -1490,7 +1629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -1506,7 +1645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -1522,7 +1661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -1538,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -1554,7 +1693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -1570,7 +1709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -1586,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -1618,7 +1757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +1773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1650,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1666,7 +1805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1682,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -1698,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1714,7 +1853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>23</v>
       </c>
@@ -1730,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>23</v>
       </c>
@@ -1746,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -1762,7 +1901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1778,7 +1917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -1794,7 +1933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -1810,7 +1949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -1826,7 +1965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -1842,7 +1981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -1858,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +2013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +2029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -1906,7 +2045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -1922,7 +2061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -1938,7 +2077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -1954,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -1970,7 +2109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -1986,7 +2125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2002,7 +2141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -2018,7 +2157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -2034,7 +2173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -2050,7 +2189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -2066,7 +2205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -2082,7 +2221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
finalized visualisation, tidy rmd, ready for doc
</commit_message>
<xml_diff>
--- a/code/data/Edge_List_Transfers.xlsx
+++ b/code/data/Edge_List_Transfers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\Studium\Master\4_Semester\MethodenDerSozialenNetzwerke\Project\SocialNetworkAnalysis\social_network_analysis\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8776A4-CE94-4A30-86D9-4E1C84713FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D2BBBE-000A-4F48-AD2D-C2AFEDA8D590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2115" yWindow="2280" windowWidth="43200" windowHeight="12735" xr2:uid="{FABA5661-431C-7B4B-8938-D299ED5A487A}"/>
   </bookViews>
@@ -588,7 +588,7 @@
   <dimension ref="A1:S93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="G1" sqref="G1:G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Heimarbeit2 completed including pdf
</commit_message>
<xml_diff>
--- a/code/data/Edge_List_Transfers.xlsx
+++ b/code/data/Edge_List_Transfers.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\Studium\Master\4_Semester\MethodenDerSozialenNetzwerke\Project\SocialNetworkAnalysis\social_network_analysis\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D2BBBE-000A-4F48-AD2D-C2AFEDA8D590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5379B0D8-DE6B-45C9-8AA3-13EE931EEB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2280" windowWidth="43200" windowHeight="12735" xr2:uid="{FABA5661-431C-7B4B-8938-D299ED5A487A}"/>
+    <workbookView xWindow="2115" yWindow="2280" windowWidth="43200" windowHeight="12735" activeTab="2" xr2:uid="{FABA5661-431C-7B4B-8938-D299ED5A487A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Type" sheetId="2" r:id="rId2"/>
+    <sheet name="Teams" sheetId="3" r:id="rId2"/>
+    <sheet name="SuperLeague" sheetId="4" r:id="rId3"/>
+    <sheet name="Challenge League" sheetId="5" r:id="rId4"/>
+    <sheet name="Type" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="63">
   <si>
     <t>Kürzel x</t>
   </si>
@@ -210,6 +213,21 @@
   </si>
   <si>
     <t>TypeID</t>
+  </si>
+  <si>
+    <t>Super League</t>
+  </si>
+  <si>
+    <t>Challenge League</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team </t>
+  </si>
+  <si>
+    <t>Kuerzel</t>
+  </si>
+  <si>
+    <t>Liga</t>
   </si>
 </sst>
 </file>
@@ -587,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ACF79-FBB0-FD4B-BB40-44B82F9281BB}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G93"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4048,6 +4066,464 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFB31FC-56C6-46C4-85E4-5E0AC51AB8D0}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D464C1-6BC3-4860-9255-FEFE1035EBC3}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12CD5CE-E72C-4FBB-8123-ED4312441C9C}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909BAF0D-EF04-4E7C-8130-A0509904D1C1}">
   <dimension ref="A1:B93"/>
   <sheetViews>

</xml_diff>